<commit_message>
more procs, not used anymore?
</commit_message>
<xml_diff>
--- a/buildtool/procs.xlsx
+++ b/buildtool/procs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1416" yWindow="0" windowWidth="21624" windowHeight="9984"/>
+    <workbookView xWindow="2820" yWindow="0" windowWidth="20220" windowHeight="9972"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Procname</t>
   </si>
@@ -63,6 +63,15 @@
   </si>
   <si>
     <t>?</t>
+  </si>
+  <si>
+    <t>report_summary_testrun</t>
+  </si>
+  <si>
+    <t>./perftools/report/report-run-dir.tcl</t>
+  </si>
+  <si>
+    <t>[2017-04-03 11:03:30] Deze zou nu niet meer nodig moeten zijn, met stacktraces aanvulling, zie ndv::source_once.tcl</t>
   </si>
 </sst>
 </file>
@@ -359,12 +368,12 @@
   <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="50.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -419,6 +428,19 @@
         <v>12</v>
       </c>
     </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+    </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" s="2"/>
     </row>

</xml_diff>